<commit_message>
Commit Changes to Selenium advance Framework
</commit_message>
<xml_diff>
--- a/excel/testdata.xlsx
+++ b/excel/testdata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>testname</t>
   </si>
@@ -57,15 +57,15 @@
     <t>1</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>newTest</t>
   </si>
   <si>
     <t>To check wheter this test is executed</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
@@ -81,40 +81,37 @@
     <t>yes</t>
   </si>
   <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
+  </si>
+  <si>
+    <t>amuthan</t>
+  </si>
+  <si>
+    <t>testing Neosoft Technology</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Meetings</t>
+  </si>
+  <si>
+    <t>Web Werks</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Faraz</t>
+  </si>
+  <si>
     <t>edge</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>amuthan</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>testing Neosoft Technology</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Admin123</t>
-  </si>
-  <si>
-    <t>subscribe</t>
-  </si>
-  <si>
-    <t>Web Werks</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Faraz</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1067,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1113,21 +1110,21 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -1142,19 +1139,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="15.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="8.14285714285714" customWidth="1"/>
     <col min="3" max="3" width="8.28571428571429" customWidth="1"/>
     <col min="4" max="4" width="9.85714285714286" customWidth="1"/>
-    <col min="5" max="5" width="9.57142857142857" customWidth="1"/>
+    <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="27.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1185,7 +1182,7 @@
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1205,8 +1202,8 @@
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
@@ -1215,7 +1212,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1223,19 +1220,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1243,10 +1240,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
@@ -1255,18 +1252,18 @@
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
@@ -1274,19 +1271,19 @@
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>27</v>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>18</v>
@@ -1294,8 +1291,8 @@
       <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1303,19 +1300,99 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commited by Faraz Dasurkar Binary Files Updated in Driver.
</commit_message>
<xml_diff>
--- a/excel/testdata.xlsx
+++ b/excel/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620"/>
+    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DATA" sheetId="3" r:id="rId2"/>
+    <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>testname</t>
   </si>
@@ -45,10 +45,10 @@
     <t>count</t>
   </si>
   <si>
-    <t>loginlogout</t>
-  </si>
-  <si>
-    <t>To check wheter the user can successfully login and logout</t>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>To check wheter this test is executed</t>
   </si>
   <si>
     <t>Yes</t>
@@ -57,10 +57,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>newTest</t>
-  </si>
-  <si>
-    <t>To check wheter this test is executed</t>
+    <t>Searchproduct</t>
+  </si>
+  <si>
+    <t>Tseach prodcusct</t>
   </si>
   <si>
     <t>2</t>
@@ -91,27 +91,6 @@
   </si>
   <si>
     <t>amuthan</t>
-  </si>
-  <si>
-    <t>testing Neosoft Technology</t>
-  </si>
-  <si>
-    <t>Firefox</t>
-  </si>
-  <si>
-    <t>Meetings</t>
-  </si>
-  <si>
-    <t>Web Werks</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Faraz</t>
-  </si>
-  <si>
-    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -124,13 +103,27 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0066CC"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -277,12 +270,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -610,141 +609,146 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,7 +827,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -835,7 +839,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -852,9 +856,9 @@
         <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -887,9 +891,9 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1064,69 +1068,83 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="15.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="53.7142857142857" customWidth="1"/>
-    <col min="3" max="4" width="10.1428571428571" customWidth="1"/>
-    <col min="8" max="8" width="13.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="1" max="1" width="14.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="37.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1139,20 +1157,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="15.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="8.14285714285714" customWidth="1"/>
-    <col min="3" max="3" width="8.28571428571429" customWidth="1"/>
-    <col min="4" max="4" width="9.85714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="8.71428571428571" customWidth="1"/>
+    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
+    <col min="4" max="4" width="10.4285714285714" customWidth="1"/>
     <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="27.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="9.42857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1176,227 +1194,67 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commited by faraz Dasurkar
</commit_message>
<xml_diff>
--- a/excel/testdata.xlsx
+++ b/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView windowWidth="21600" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="48">
   <si>
     <t>testname</t>
   </si>
@@ -45,10 +45,10 @@
     <t>count</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>To check wheter this test is executed</t>
+    <t>Milksearchproduct</t>
+  </si>
+  <si>
+    <t>will search milk products here</t>
   </si>
   <si>
     <t>Yes</t>
@@ -57,46 +57,121 @@
     <t>1</t>
   </si>
   <si>
-    <t>Searchproduct</t>
-  </si>
-  <si>
-    <t>Tseach prodcusct</t>
+    <t>Rusksearchproduct</t>
+  </si>
+  <si>
+    <t>This is just a landing page</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
+    <t>Onionsearchproduct</t>
+  </si>
+  <si>
+    <t>will search onion here</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>detergentsearchproduct</t>
+  </si>
+  <si>
+    <t>will search detergent powder here</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>searchcookoil</t>
+  </si>
+  <si>
+    <t>will search fortune oil here</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>softdrink</t>
+  </si>
+  <si>
+    <t>will search softdrink here</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>aata</t>
+  </si>
+  <si>
+    <t>will search aata here</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>tatatea</t>
+  </si>
+  <si>
+    <t>will search tatatea here</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>browser</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>product</t>
+  </si>
+  <si>
+    <t>SecondProduct</t>
   </si>
   <si>
     <t>Chrome</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>YWRtaW4xMjM=</t>
-  </si>
-  <si>
-    <t>amuthan</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>Rusk</t>
+  </si>
+  <si>
+    <t>Britania Rusk</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Amul Masti Dahi Pouch</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>surf excel</t>
+  </si>
+  <si>
+    <t>Fortune oil</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>atta</t>
+  </si>
+  <si>
+    <t>Atta</t>
+  </si>
+  <si>
+    <t>Tata Agni Leaf Tea Pouch</t>
   </si>
   <si>
     <t>Edge</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -104,10 +179,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -127,7 +202,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0066CC"/>
+      <color rgb="FF000000"/>
       <name val="Consolas"/>
       <charset val="134"/>
     </font>
@@ -603,16 +678,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -745,16 +820,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,15 +1156,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="22.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="37.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1104,36 +1186,138 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1146,23 +1330,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="21.7809523809524" customWidth="1"/>
     <col min="2" max="2" width="8.71428571428571" customWidth="1"/>
     <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
-    <col min="4" max="4" width="10.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="9.42857142857143" customWidth="1"/>
+    <col min="4" max="4" width="32.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="23.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1170,97 +1353,398 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="B23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>